<commit_message>
Sửa bổ xung Excel và xóa thành viên
</commit_message>
<xml_diff>
--- a/BiTech.Library/BiTech.Library/Tempalates/MauDDC.xlsx
+++ b/BiTech.Library/BiTech.Library/Tempalates/MauDDC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pro Test\pro2\BiTech.Library\BiTech.Library\Tempaltes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pro Test\pro2\BiTech.Library\BiTech.Library\Tempalates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -492,7 +492,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C1" activeCellId="2" sqref="A1:A1048576 B1:B1048576 C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>